<commit_message>
RESTORE v0.2: - Zenodo to CNF - CNF autoconfiguration
</commit_message>
<xml_diff>
--- a/data/zenodo_ivan/conversion/transdis/CHE_convtransdis_elec.xlsx
+++ b/data/zenodo_ivan/conversion/transdis/CHE_convtransdis_elec.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/zenodo_ivan/conversion/transdis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83A0CFD-A7DD-F64A-9A4F-AEF6A92C4285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC8CF55-1FC4-F240-AD4D-FAB2FE4AFA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17500" yWindow="500" windowWidth="20900" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="-4880" windowWidth="21600" windowHeight="37900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$L$602</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$L$603</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="42">
   <si>
     <t>Name:</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>T25. Country consumption, before transmission/distribution losses</t>
+  </si>
+  <si>
+    <t>max_activity_annual</t>
+  </si>
+  <si>
+    <t>No distribution/transmission limit</t>
   </si>
 </sst>
 </file>
@@ -574,11 +580,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L182"/>
+  <dimension ref="A1:L183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I47" sqref="I47"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -740,29 +746,21 @@
       <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" t="s">
-        <v>17</v>
+      <c r="C10" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10">
-        <v>1990</v>
-      </c>
-      <c r="G10">
-        <v>50271</v>
+        <v>23</v>
       </c>
       <c r="H10" t="s">
         <v>29</v>
       </c>
       <c r="J10" t="s">
-        <v>33</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="K10" s="2"/>
       <c r="L10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -779,10 +777,10 @@
         <v>24</v>
       </c>
       <c r="E11">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="G11">
-        <v>51336</v>
+        <v>50271</v>
       </c>
       <c r="H11" t="s">
         <v>29</v>
@@ -811,10 +809,10 @@
         <v>24</v>
       </c>
       <c r="E12">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="G12">
-        <v>51621</v>
+        <v>51336</v>
       </c>
       <c r="H12" t="s">
         <v>29</v>
@@ -843,10 +841,10 @@
         <v>24</v>
       </c>
       <c r="E13">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="G13">
-        <v>50928</v>
+        <v>51621</v>
       </c>
       <c r="H13" t="s">
         <v>29</v>
@@ -875,10 +873,10 @@
         <v>24</v>
       </c>
       <c r="E14">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="G14">
-        <v>50547</v>
+        <v>50928</v>
       </c>
       <c r="H14" t="s">
         <v>29</v>
@@ -907,10 +905,10 @@
         <v>24</v>
       </c>
       <c r="E15">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="G15">
-        <v>51567</v>
+        <v>50547</v>
       </c>
       <c r="H15" t="s">
         <v>29</v>
@@ -939,10 +937,10 @@
         <v>24</v>
       </c>
       <c r="E16">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="G16">
-        <v>52420</v>
+        <v>51567</v>
       </c>
       <c r="H16" t="s">
         <v>29</v>
@@ -971,10 +969,10 @@
         <v>24</v>
       </c>
       <c r="E17">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="G17">
-        <v>52327</v>
+        <v>52420</v>
       </c>
       <c r="H17" t="s">
         <v>29</v>
@@ -1003,10 +1001,10 @@
         <v>24</v>
       </c>
       <c r="E18">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="G18">
-        <v>53374</v>
+        <v>52327</v>
       </c>
       <c r="H18" t="s">
         <v>29</v>
@@ -1035,10 +1033,10 @@
         <v>24</v>
       </c>
       <c r="E19">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="G19">
-        <v>55056</v>
+        <v>53374</v>
       </c>
       <c r="H19" t="s">
         <v>29</v>
@@ -1067,10 +1065,10 @@
         <v>24</v>
       </c>
       <c r="E20">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="G20">
-        <v>56304</v>
+        <v>55056</v>
       </c>
       <c r="H20" t="s">
         <v>29</v>
@@ -1099,10 +1097,10 @@
         <v>24</v>
       </c>
       <c r="E21">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="G21">
-        <v>57783</v>
+        <v>56304</v>
       </c>
       <c r="H21" t="s">
         <v>29</v>
@@ -1131,10 +1129,10 @@
         <v>24</v>
       </c>
       <c r="E22">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="G22">
-        <v>58085</v>
+        <v>57783</v>
       </c>
       <c r="H22" t="s">
         <v>29</v>
@@ -1163,10 +1161,10 @@
         <v>24</v>
       </c>
       <c r="E23">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="G23">
-        <v>59261</v>
+        <v>58085</v>
       </c>
       <c r="H23" t="s">
         <v>29</v>
@@ -1195,10 +1193,10 @@
         <v>24</v>
       </c>
       <c r="E24">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="G24">
-        <v>60387</v>
+        <v>59261</v>
       </c>
       <c r="H24" t="s">
         <v>29</v>
@@ -1227,10 +1225,10 @@
         <v>24</v>
       </c>
       <c r="E25">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="G25">
-        <v>61637</v>
+        <v>60387</v>
       </c>
       <c r="H25" t="s">
         <v>29</v>
@@ -1259,10 +1257,10 @@
         <v>24</v>
       </c>
       <c r="E26">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="G26">
-        <v>62124</v>
+        <v>61637</v>
       </c>
       <c r="H26" t="s">
         <v>29</v>
@@ -1291,10 +1289,10 @@
         <v>24</v>
       </c>
       <c r="E27">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="G27">
-        <v>61750</v>
+        <v>62124</v>
       </c>
       <c r="H27" t="s">
         <v>29</v>
@@ -1323,10 +1321,10 @@
         <v>24</v>
       </c>
       <c r="E28">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="G28">
-        <v>63147</v>
+        <v>61750</v>
       </c>
       <c r="H28" t="s">
         <v>29</v>
@@ -1355,10 +1353,10 @@
         <v>24</v>
       </c>
       <c r="E29">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="G29">
-        <v>61814</v>
+        <v>63147</v>
       </c>
       <c r="H29" t="s">
         <v>29</v>
@@ -1387,10 +1385,10 @@
         <v>24</v>
       </c>
       <c r="E30">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="G30">
-        <v>64278</v>
+        <v>61814</v>
       </c>
       <c r="H30" t="s">
         <v>29</v>
@@ -1419,10 +1417,10 @@
         <v>24</v>
       </c>
       <c r="E31">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="G31">
-        <v>63002</v>
+        <v>64278</v>
       </c>
       <c r="H31" t="s">
         <v>29</v>
@@ -1451,10 +1449,10 @@
         <v>24</v>
       </c>
       <c r="E32">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="G32">
-        <v>63408</v>
+        <v>63002</v>
       </c>
       <c r="H32" t="s">
         <v>29</v>
@@ -1483,10 +1481,10 @@
         <v>24</v>
       </c>
       <c r="E33">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="G33">
-        <v>63784</v>
+        <v>63408</v>
       </c>
       <c r="H33" t="s">
         <v>29</v>
@@ -1515,10 +1513,10 @@
         <v>24</v>
       </c>
       <c r="E34">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="G34">
-        <v>61787</v>
+        <v>63784</v>
       </c>
       <c r="H34" t="s">
         <v>29</v>
@@ -1547,10 +1545,10 @@
         <v>24</v>
       </c>
       <c r="E35">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="G35">
-        <v>62626</v>
+        <v>61787</v>
       </c>
       <c r="H35" t="s">
         <v>29</v>
@@ -1579,10 +1577,10 @@
         <v>24</v>
       </c>
       <c r="E36">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="G36">
-        <v>62617</v>
+        <v>62626</v>
       </c>
       <c r="H36" t="s">
         <v>29</v>
@@ -1611,10 +1609,10 @@
         <v>24</v>
       </c>
       <c r="E37">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="G37">
-        <v>62877</v>
+        <v>62617</v>
       </c>
       <c r="H37" t="s">
         <v>29</v>
@@ -1643,10 +1641,10 @@
         <v>24</v>
       </c>
       <c r="E38">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="G38">
-        <v>61984</v>
+        <v>62877</v>
       </c>
       <c r="H38" t="s">
         <v>29</v>
@@ -1675,10 +1673,10 @@
         <v>24</v>
       </c>
       <c r="E39">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="G39">
-        <v>61501</v>
+        <v>61984</v>
       </c>
       <c r="H39" t="s">
         <v>29</v>
@@ -1701,25 +1699,28 @@
         <v>37</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D40" t="s">
         <v>24</v>
       </c>
       <c r="E40">
-        <v>1990</v>
+        <v>2019</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>61501</v>
       </c>
       <c r="H40" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="J40" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="L40" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
@@ -1736,7 +1737,7 @@
         <v>24</v>
       </c>
       <c r="E41">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -1765,7 +1766,7 @@
         <v>24</v>
       </c>
       <c r="E42">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -1794,7 +1795,7 @@
         <v>24</v>
       </c>
       <c r="E43">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -1823,7 +1824,7 @@
         <v>24</v>
       </c>
       <c r="E44">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -1852,7 +1853,7 @@
         <v>24</v>
       </c>
       <c r="E45">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -1881,7 +1882,7 @@
         <v>24</v>
       </c>
       <c r="E46">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -1910,7 +1911,7 @@
         <v>24</v>
       </c>
       <c r="E47">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -1939,7 +1940,7 @@
         <v>24</v>
       </c>
       <c r="E48">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -1968,7 +1969,7 @@
         <v>24</v>
       </c>
       <c r="E49">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -1997,7 +1998,7 @@
         <v>24</v>
       </c>
       <c r="E50">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -2026,7 +2027,7 @@
         <v>24</v>
       </c>
       <c r="E51">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -2055,7 +2056,7 @@
         <v>24</v>
       </c>
       <c r="E52">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -2084,7 +2085,7 @@
         <v>24</v>
       </c>
       <c r="E53">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -2113,7 +2114,7 @@
         <v>24</v>
       </c>
       <c r="E54">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -2142,7 +2143,7 @@
         <v>24</v>
       </c>
       <c r="E55">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -2171,7 +2172,7 @@
         <v>24</v>
       </c>
       <c r="E56">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -2200,7 +2201,7 @@
         <v>24</v>
       </c>
       <c r="E57">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -2229,7 +2230,7 @@
         <v>24</v>
       </c>
       <c r="E58">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -2258,7 +2259,7 @@
         <v>24</v>
       </c>
       <c r="E59">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -2287,7 +2288,7 @@
         <v>24</v>
       </c>
       <c r="E60">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -2316,7 +2317,7 @@
         <v>24</v>
       </c>
       <c r="E61">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -2345,7 +2346,7 @@
         <v>24</v>
       </c>
       <c r="E62">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -2374,7 +2375,7 @@
         <v>24</v>
       </c>
       <c r="E63">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -2403,7 +2404,7 @@
         <v>24</v>
       </c>
       <c r="E64">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -2432,7 +2433,7 @@
         <v>24</v>
       </c>
       <c r="E65">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -2461,7 +2462,7 @@
         <v>24</v>
       </c>
       <c r="E66">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -2490,7 +2491,7 @@
         <v>24</v>
       </c>
       <c r="E67">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -2519,7 +2520,7 @@
         <v>24</v>
       </c>
       <c r="E68">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -2548,30 +2549,59 @@
         <v>24</v>
       </c>
       <c r="E69">
+        <v>2018</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69" t="s">
+        <v>35</v>
+      </c>
+      <c r="J69" t="s">
+        <v>28</v>
+      </c>
+      <c r="L69" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>16</v>
+      </c>
+      <c r="B70" t="s">
+        <v>37</v>
+      </c>
+      <c r="C70" t="s">
+        <v>19</v>
+      </c>
+      <c r="D70" t="s">
+        <v>24</v>
+      </c>
+      <c r="E70">
         <v>2019</v>
       </c>
-      <c r="G69">
-        <v>0</v>
-      </c>
-      <c r="H69" t="s">
-        <v>35</v>
-      </c>
-      <c r="J69" t="s">
-        <v>28</v>
-      </c>
-      <c r="L69" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="182" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K182" s="2"/>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70" t="s">
+        <v>35</v>
+      </c>
+      <c r="J70" t="s">
+        <v>28</v>
+      </c>
+      <c r="L70" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="183" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K183" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:L602" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A5:L603" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1" xr:uid="{F043F192-E5FA-F046-BD61-2DE7DC685D42}"/>
-    <hyperlink ref="K11:K39" r:id="rId2" display="https://www.bfe.admin.ch/bfe/fr/home/approvisionnement/statistiques-et-geodonnees/statistiques-de-lenergie/statistique-globale-de-l-energie.html/" xr:uid="{6FEF95C0-6A4A-4848-ABF7-D80895B93980}"/>
+    <hyperlink ref="K11" r:id="rId1" xr:uid="{F043F192-E5FA-F046-BD61-2DE7DC685D42}"/>
+    <hyperlink ref="K12:K40" r:id="rId2" display="https://www.bfe.admin.ch/bfe/fr/home/approvisionnement/statistiques-et-geodonnees/statistiques-de-lenergie/statistique-globale-de-l-energie.html/" xr:uid="{6FEF95C0-6A4A-4848-ABF7-D80895B93980}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>